<commit_message>
Newly added script 2nd time
</commit_message>
<xml_diff>
--- a/DemoTest/src/test/resources/testdata/exceldata.xlsx
+++ b/DemoTest/src/test/resources/testdata/exceldata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9D2F00BA-AB27-411C-9B36-CBE0DF75F882}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2F8F27AD-FBEA-4943-A4FE-26CC79D86959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="2535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="2535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>F</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Sangeethapriya</t>
+  </si>
+  <si>
+    <t>P R</t>
+  </si>
+  <si>
+    <t>stest@gmail.com</t>
+  </si>
+  <si>
+    <t>Stest@123</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Priyas@gmail.com</t>
+  </si>
+  <si>
+    <t>priyanew@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,13 +85,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -344,23 +373,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{ABE23351-2F79-40B5-AE69-B1FB64342C4E}"/>
+    <hyperlink ref="E1" r:id="rId2" xr:uid="{1B33F0B7-5E75-4D2D-987B-095FE2D66FBC}"/>
+    <hyperlink ref="F1" r:id="rId3" xr:uid="{9FBADCA3-2B22-42CB-B031-E773EC3E6B94}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{4EBEAEF8-7641-4F40-8F06-D475D7A9FCE8}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{AEFD8F4F-1A88-4EA2-BDF8-649041052F35}"/>
+    <hyperlink ref="F2" r:id="rId6" xr:uid="{3626173F-C01F-4C8D-999A-1A0F3BA4E6A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mvn cmd and jenkins add script name as _Test
</commit_message>
<xml_diff>
--- a/DemoTest/src/test/resources/testdata/exceldata.xlsx
+++ b/DemoTest/src/test/resources/testdata/exceldata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2F8F27AD-FBEA-4943-A4FE-26CC79D86959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{891A73D5-746C-4839-8768-EC5675523F75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="2535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6450" windowHeight="2535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,16 +35,16 @@
     <t>Stest@123</t>
   </si>
   <si>
-    <t>Priya</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Priyas@gmail.com</t>
-  </si>
-  <si>
     <t>priyanew@123</t>
+  </si>
+  <si>
+    <t>Priyaspr1</t>
+  </si>
+  <si>
+    <t>SPRPriyas@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,19 +400,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>